<commit_message>
Integrated a split function
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Sale Number</t>
   </si>
@@ -43,13 +43,13 @@
     <t xml:space="preserve">2025 Evan Drilhet </t>
   </si>
   <si>
-    <t>23 Mom</t>
+    <t>23 Mom, ryan</t>
   </si>
   <si>
     <t>Thomas Whitson Freshman</t>
   </si>
   <si>
-    <t>Drew Bevington Senior</t>
+    <t>Drew Bevington Senior, ryan, mom, trevor</t>
   </si>
   <si>
     <t>Sasha Stella 2024</t>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">2024 Chloe Atha </t>
+  </si>
+  <si>
+    <t>Trevor John, Drew, Chloe</t>
   </si>
 </sst>
 </file>
@@ -546,7 +549,7 @@
         <v>0.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3">
         <v>23.0</v>

</xml_diff>